<commit_message>
Updated with example data
</commit_message>
<xml_diff>
--- a/Equipment Inventory.xlsx
+++ b/Equipment Inventory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ronnie\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ronnie\Desktop\SD\MCNF\SDTeam21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34E0C3E-1CF5-4C9E-97FD-B5F4AE23B42E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CE1DE4-13AB-48F5-8D17-5BA491F4186E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2580" windowWidth="14400" windowHeight="7360" firstSheet="2" activeTab="4" xr2:uid="{73C4247B-C753-4CD8-90B0-421248CE9046}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{73C4247B-C753-4CD8-90B0-421248CE9046}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory by Room" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,13 @@
     <sheet name="Storage Rooms" sheetId="3" r:id="rId4"/>
     <sheet name="Event Requirements" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Commodities!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Event Requirements'!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Inventory by Commodity'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Inventory by Room'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Storage Rooms'!$A$1:$H$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
   <si>
     <t>Storage Room</t>
   </si>
@@ -49,9 +56,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Volume/unity</t>
-  </si>
-  <si>
     <t>Volume/Parcel</t>
   </si>
   <si>
@@ -64,9 +68,6 @@
     <t>Capacity Factor</t>
   </si>
   <si>
-    <t>S1</t>
-  </si>
-  <si>
     <t>Physical Capacity (sqft)</t>
   </si>
   <si>
@@ -79,9 +80,6 @@
     <t>At Capacity (1,0,-1)</t>
   </si>
   <si>
-    <t>Fill</t>
-  </si>
-  <si>
     <t>Event</t>
   </si>
   <si>
@@ -101,14 +99,105 @@
   </si>
   <si>
     <t>Equipment Type</t>
+  </si>
+  <si>
+    <t>S 01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chairs </t>
+  </si>
+  <si>
+    <t>Tables</t>
+  </si>
+  <si>
+    <t>Chairs</t>
+  </si>
+  <si>
+    <t>S 02</t>
+  </si>
+  <si>
+    <r>
+      <t>1 / m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2 / m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>Parcel Size</t>
+  </si>
+  <si>
+    <t>Nominal Fill</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Council of Supply Chain Management</t>
+  </si>
+  <si>
+    <t>C 205</t>
+  </si>
+  <si>
+    <t>MEETING ROOM CHAIRS</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>C 210</t>
+  </si>
+  <si>
+    <t>66" ROUND TABLES</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -136,9 +225,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,19 +544,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB62A666-68AE-4237-AC87-E578B4BA207A}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,23 +572,59 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" s="2">
+        <v>43535</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2">
+        <v>43535</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K8" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:D1" xr:uid="{9E4999E4-082B-42E9-8175-DB32C7C4B1CE}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F9A5E4-2E63-489F-BF3F-C8ADE7EE1010}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -512,24 +641,54 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" s="2">
+        <v>43535</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>110</v>
+      </c>
+      <c r="D3" s="2">
+        <v>43535</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:D1" xr:uid="{E84D4C31-3FAF-4B48-A5F7-E652144DA016}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09ECBFA8-7437-4CB4-A947-A458D852B66B}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -537,35 +696,58 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3">
         <v>5</v>
       </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{622EDA50-4933-4C28-9537-A85F854DBF51}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D720228-430F-4D49-85BD-9810C22B4911}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.36328125" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -573,30 +755,30 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -609,7 +791,7 @@
         <v>90</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" t="e">
         <f>E2/D2</f>
@@ -619,52 +801,211 @@
         <f>E2-D2</f>
         <v>#VALUE!</v>
       </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>900</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="D3">
+        <f>ROUND(B3*C3, 1)</f>
+        <v>765</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="e">
+        <f>E3/D3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G3" t="e">
+        <f>E3-D3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H1" xr:uid="{4C616255-1A36-4DCB-878C-A63A1AB7987C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C54136F-60C6-44C7-88F8-939D93B3E246}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" t="s">
-        <v>21</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
       </c>
+      <c r="I1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="3">
+        <v>43000</v>
+      </c>
+      <c r="D2" s="3">
+        <v>43000.416666666664</v>
+      </c>
+      <c r="E2" s="3">
+        <v>43003.4375</v>
+      </c>
+      <c r="F2" s="3">
+        <v>43004.708333333336</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2">
+        <v>225</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="3">
+        <v>43000</v>
+      </c>
+      <c r="D3" s="3">
+        <v>43000.416666666664</v>
+      </c>
+      <c r="E3" s="3">
+        <v>43003.4375</v>
+      </c>
+      <c r="F3" s="3">
+        <v>43004.708333333336</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="3">
+        <v>43000</v>
+      </c>
+      <c r="D4" s="3">
+        <v>43000.416666666664</v>
+      </c>
+      <c r="E4" s="3">
+        <v>43003.4375</v>
+      </c>
+      <c r="F4" s="3">
+        <v>43004.708333333336</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4">
+        <v>225</v>
+      </c>
+      <c r="I4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3">
+        <v>43000</v>
+      </c>
+      <c r="D5" s="3">
+        <v>43000.416666666664</v>
+      </c>
+      <c r="E5" s="3">
+        <v>43003.4375</v>
+      </c>
+      <c r="F5" s="3">
+        <v>43004.708333333336</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5">
+        <v>9</v>
+      </c>
+      <c r="I5" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I1" xr:uid="{817BECB0-BF98-45CD-9F72-C0680053F0EB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added excel reading and split output into 4 disjoint sets
</commit_message>
<xml_diff>
--- a/Equipment Inventory.xlsx
+++ b/Equipment Inventory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ronnie\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ronnie\Desktop\SD\MCNF\SDTeam21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34E0C3E-1CF5-4C9E-97FD-B5F4AE23B42E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CE1DE4-13AB-48F5-8D17-5BA491F4186E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2580" windowWidth="14400" windowHeight="7360" firstSheet="2" activeTab="4" xr2:uid="{73C4247B-C753-4CD8-90B0-421248CE9046}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{73C4247B-C753-4CD8-90B0-421248CE9046}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory by Room" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,13 @@
     <sheet name="Storage Rooms" sheetId="3" r:id="rId4"/>
     <sheet name="Event Requirements" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Commodities!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Event Requirements'!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Inventory by Commodity'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Inventory by Room'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Storage Rooms'!$A$1:$H$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
   <si>
     <t>Storage Room</t>
   </si>
@@ -49,9 +56,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Volume/unity</t>
-  </si>
-  <si>
     <t>Volume/Parcel</t>
   </si>
   <si>
@@ -64,9 +68,6 @@
     <t>Capacity Factor</t>
   </si>
   <si>
-    <t>S1</t>
-  </si>
-  <si>
     <t>Physical Capacity (sqft)</t>
   </si>
   <si>
@@ -79,9 +80,6 @@
     <t>At Capacity (1,0,-1)</t>
   </si>
   <si>
-    <t>Fill</t>
-  </si>
-  <si>
     <t>Event</t>
   </si>
   <si>
@@ -101,14 +99,105 @@
   </si>
   <si>
     <t>Equipment Type</t>
+  </si>
+  <si>
+    <t>S 01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chairs </t>
+  </si>
+  <si>
+    <t>Tables</t>
+  </si>
+  <si>
+    <t>Chairs</t>
+  </si>
+  <si>
+    <t>S 02</t>
+  </si>
+  <si>
+    <r>
+      <t>1 / m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2 / m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>Parcel Size</t>
+  </si>
+  <si>
+    <t>Nominal Fill</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Council of Supply Chain Management</t>
+  </si>
+  <si>
+    <t>C 205</t>
+  </si>
+  <si>
+    <t>MEETING ROOM CHAIRS</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>C 210</t>
+  </si>
+  <si>
+    <t>66" ROUND TABLES</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -136,9 +225,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,19 +544,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB62A666-68AE-4237-AC87-E578B4BA207A}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,23 +572,59 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" s="2">
+        <v>43535</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2">
+        <v>43535</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K8" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:D1" xr:uid="{9E4999E4-082B-42E9-8175-DB32C7C4B1CE}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F9A5E4-2E63-489F-BF3F-C8ADE7EE1010}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -512,24 +641,54 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" s="2">
+        <v>43535</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>110</v>
+      </c>
+      <c r="D3" s="2">
+        <v>43535</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:D1" xr:uid="{E84D4C31-3FAF-4B48-A5F7-E652144DA016}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09ECBFA8-7437-4CB4-A947-A458D852B66B}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -537,35 +696,58 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3">
         <v>5</v>
       </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{622EDA50-4933-4C28-9537-A85F854DBF51}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D720228-430F-4D49-85BD-9810C22B4911}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.36328125" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -573,30 +755,30 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -609,7 +791,7 @@
         <v>90</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" t="e">
         <f>E2/D2</f>
@@ -619,52 +801,211 @@
         <f>E2-D2</f>
         <v>#VALUE!</v>
       </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>900</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="D3">
+        <f>ROUND(B3*C3, 1)</f>
+        <v>765</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="e">
+        <f>E3/D3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G3" t="e">
+        <f>E3-D3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H1" xr:uid="{4C616255-1A36-4DCB-878C-A63A1AB7987C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C54136F-60C6-44C7-88F8-939D93B3E246}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" t="s">
-        <v>21</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
       </c>
+      <c r="I1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="3">
+        <v>43000</v>
+      </c>
+      <c r="D2" s="3">
+        <v>43000.416666666664</v>
+      </c>
+      <c r="E2" s="3">
+        <v>43003.4375</v>
+      </c>
+      <c r="F2" s="3">
+        <v>43004.708333333336</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2">
+        <v>225</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="3">
+        <v>43000</v>
+      </c>
+      <c r="D3" s="3">
+        <v>43000.416666666664</v>
+      </c>
+      <c r="E3" s="3">
+        <v>43003.4375</v>
+      </c>
+      <c r="F3" s="3">
+        <v>43004.708333333336</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="3">
+        <v>43000</v>
+      </c>
+      <c r="D4" s="3">
+        <v>43000.416666666664</v>
+      </c>
+      <c r="E4" s="3">
+        <v>43003.4375</v>
+      </c>
+      <c r="F4" s="3">
+        <v>43004.708333333336</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4">
+        <v>225</v>
+      </c>
+      <c r="I4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3">
+        <v>43000</v>
+      </c>
+      <c r="D5" s="3">
+        <v>43000.416666666664</v>
+      </c>
+      <c r="E5" s="3">
+        <v>43003.4375</v>
+      </c>
+      <c r="F5" s="3">
+        <v>43004.708333333336</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5">
+        <v>9</v>
+      </c>
+      <c r="I5" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I1" xr:uid="{817BECB0-BF98-45CD-9F72-C0680053F0EB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>